<commit_message>
update instruction enum with new mnemonics and variants
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Code\chip16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\chip16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5E52FE0-D2CA-47AD-B0FA-9DF648F91301}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B5B0B0-D2AA-4CCC-AAD9-E52C10523843}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{46DFD0A6-98B0-40CA-87AE-5F9AE7027D73}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{46DFD0A6-98B0-40CA-87AE-5F9AE7027D73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="instructions_old" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="388">
   <si>
     <t>00 00 00 00</t>
   </si>
@@ -1063,6 +1064,132 @@
   </si>
   <si>
     <t>NEG1</t>
+  </si>
+  <si>
+    <t>DRWI</t>
+  </si>
+  <si>
+    <t>DRWR</t>
+  </si>
+  <si>
+    <t>JMPI</t>
+  </si>
+  <si>
+    <t>CALLI</t>
+  </si>
+  <si>
+    <t>JMPR</t>
+  </si>
+  <si>
+    <t>CALLR</t>
+  </si>
+  <si>
+    <t>LDIR</t>
+  </si>
+  <si>
+    <t>LDIS</t>
+  </si>
+  <si>
+    <t>LDMI</t>
+  </si>
+  <si>
+    <t>LDMR</t>
+  </si>
+  <si>
+    <t>STMI</t>
+  </si>
+  <si>
+    <t>STMR</t>
+  </si>
+  <si>
+    <t>ADDR2</t>
+  </si>
+  <si>
+    <t>ADDR3</t>
+  </si>
+  <si>
+    <t>SUBR2</t>
+  </si>
+  <si>
+    <t>SUBR3</t>
+  </si>
+  <si>
+    <t>ANDR2</t>
+  </si>
+  <si>
+    <t>ANDR3</t>
+  </si>
+  <si>
+    <t>ORR2</t>
+  </si>
+  <si>
+    <t>ORR3</t>
+  </si>
+  <si>
+    <t>XORR2</t>
+  </si>
+  <si>
+    <t>XORR3</t>
+  </si>
+  <si>
+    <t>MULR2</t>
+  </si>
+  <si>
+    <t>MULR3</t>
+  </si>
+  <si>
+    <t>DIVR2</t>
+  </si>
+  <si>
+    <t>DIVR3</t>
+  </si>
+  <si>
+    <t>MODR2</t>
+  </si>
+  <si>
+    <t>MODR3</t>
+  </si>
+  <si>
+    <t>REMR2</t>
+  </si>
+  <si>
+    <t>REMR3</t>
+  </si>
+  <si>
+    <t>PALI</t>
+  </si>
+  <si>
+    <t>PALR</t>
+  </si>
+  <si>
+    <t>NOTR1</t>
+  </si>
+  <si>
+    <t>NOTR2</t>
+  </si>
+  <si>
+    <t>NEGR1</t>
+  </si>
+  <si>
+    <t>NEGR2</t>
+  </si>
+  <si>
+    <t>SHLN</t>
+  </si>
+  <si>
+    <t>SHRN</t>
+  </si>
+  <si>
+    <t>SARN</t>
+  </si>
+  <si>
+    <t>SHLR</t>
+  </si>
+  <si>
+    <t>SHRR</t>
+  </si>
+  <si>
+    <t>SARR</t>
   </si>
 </sst>
 </file>
@@ -1086,12 +1213,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1106,24 +1239,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1464,10 +1589,1637 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC7A0C0-42A8-44E9-A132-FD9D5B04F362}">
+  <dimension ref="A1:F86"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>349</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>350</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>280</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>351</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>352</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>353</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>354</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>355</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>281</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" t="s">
+        <v>356</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>357</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D37" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D41" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D44" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" t="s">
+        <v>287</v>
+      </c>
+      <c r="D47" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" t="s">
+        <v>288</v>
+      </c>
+      <c r="D48" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>289</v>
+      </c>
+      <c r="D49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" t="s">
+        <v>135</v>
+      </c>
+      <c r="F49">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>364</v>
+      </c>
+      <c r="D50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="s">
+        <v>365</v>
+      </c>
+      <c r="D51" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F51">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" t="s">
+        <v>290</v>
+      </c>
+      <c r="D52" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s">
+        <v>366</v>
+      </c>
+      <c r="D53" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" t="s">
+        <v>367</v>
+      </c>
+      <c r="D54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" t="s">
+        <v>291</v>
+      </c>
+      <c r="D55" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" t="s">
+        <v>169</v>
+      </c>
+      <c r="F55">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" t="s">
+        <v>368</v>
+      </c>
+      <c r="D56" t="s">
+        <v>175</v>
+      </c>
+      <c r="E56" t="s">
+        <v>169</v>
+      </c>
+      <c r="F56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" t="s">
+        <v>369</v>
+      </c>
+      <c r="D57" t="s">
+        <v>176</v>
+      </c>
+      <c r="E57" t="s">
+        <v>169</v>
+      </c>
+      <c r="F57">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" t="s">
+        <v>292</v>
+      </c>
+      <c r="D58" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" t="s">
+        <v>370</v>
+      </c>
+      <c r="D59" t="s">
+        <v>196</v>
+      </c>
+      <c r="E59" t="s">
+        <v>169</v>
+      </c>
+      <c r="F59">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" t="s">
+        <v>371</v>
+      </c>
+      <c r="D60" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" t="s">
+        <v>135</v>
+      </c>
+      <c r="F61">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>185</v>
+      </c>
+      <c r="B62" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" t="s">
+        <v>372</v>
+      </c>
+      <c r="D62" t="s">
+        <v>199</v>
+      </c>
+      <c r="E62" t="s">
+        <v>135</v>
+      </c>
+      <c r="F62">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>187</v>
+      </c>
+      <c r="B63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" t="s">
+        <v>373</v>
+      </c>
+      <c r="D63" t="s">
+        <v>200</v>
+      </c>
+      <c r="E63" t="s">
+        <v>135</v>
+      </c>
+      <c r="F63">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
+        <v>325</v>
+      </c>
+      <c r="D64" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>135</v>
+      </c>
+      <c r="F64">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" t="s">
+        <v>374</v>
+      </c>
+      <c r="D65" t="s">
+        <v>202</v>
+      </c>
+      <c r="E65" t="s">
+        <v>135</v>
+      </c>
+      <c r="F65">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>375</v>
+      </c>
+      <c r="D66" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" t="s">
+        <v>135</v>
+      </c>
+      <c r="F66">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" t="s">
+        <v>205</v>
+      </c>
+      <c r="C67" t="s">
+        <v>382</v>
+      </c>
+      <c r="D67" t="s">
+        <v>218</v>
+      </c>
+      <c r="E67" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" t="s">
+        <v>383</v>
+      </c>
+      <c r="D68" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" t="s">
+        <v>384</v>
+      </c>
+      <c r="D69" t="s">
+        <v>220</v>
+      </c>
+      <c r="E69" t="s">
+        <v>135</v>
+      </c>
+      <c r="F69">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>211</v>
+      </c>
+      <c r="B70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" t="s">
+        <v>385</v>
+      </c>
+      <c r="D70" t="s">
+        <v>221</v>
+      </c>
+      <c r="E70" t="s">
+        <v>135</v>
+      </c>
+      <c r="F70">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
+        <v>386</v>
+      </c>
+      <c r="D71" t="s">
+        <v>222</v>
+      </c>
+      <c r="E71" t="s">
+        <v>135</v>
+      </c>
+      <c r="F71">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>216</v>
+      </c>
+      <c r="B72" t="s">
+        <v>217</v>
+      </c>
+      <c r="C72" t="s">
+        <v>387</v>
+      </c>
+      <c r="D72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" t="s">
+        <v>135</v>
+      </c>
+      <c r="F72">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" t="s">
+        <v>336</v>
+      </c>
+      <c r="D73" t="s">
+        <v>236</v>
+      </c>
+      <c r="F73">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" t="s">
+        <v>227</v>
+      </c>
+      <c r="C74" t="s">
+        <v>337</v>
+      </c>
+      <c r="D74" t="s">
+        <v>237</v>
+      </c>
+      <c r="F74">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>228</v>
+      </c>
+      <c r="B75" t="s">
+        <v>229</v>
+      </c>
+      <c r="C75" t="s">
+        <v>229</v>
+      </c>
+      <c r="D75" t="s">
+        <v>238</v>
+      </c>
+      <c r="F75">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" t="s">
+        <v>231</v>
+      </c>
+      <c r="D76" t="s">
+        <v>239</v>
+      </c>
+      <c r="F76">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" t="s">
+        <v>233</v>
+      </c>
+      <c r="D77" t="s">
+        <v>240</v>
+      </c>
+      <c r="F77">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>234</v>
+      </c>
+      <c r="B78" t="s">
+        <v>235</v>
+      </c>
+      <c r="C78" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" t="s">
+        <v>241</v>
+      </c>
+      <c r="F78">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>242</v>
+      </c>
+      <c r="B79" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" t="s">
+        <v>376</v>
+      </c>
+      <c r="D79" t="s">
+        <v>246</v>
+      </c>
+      <c r="F79">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>244</v>
+      </c>
+      <c r="B80" t="s">
+        <v>245</v>
+      </c>
+      <c r="C80" t="s">
+        <v>377</v>
+      </c>
+      <c r="D80" t="s">
+        <v>247</v>
+      </c>
+      <c r="F80">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>248</v>
+      </c>
+      <c r="B81" t="s">
+        <v>249</v>
+      </c>
+      <c r="C81" t="s">
+        <v>340</v>
+      </c>
+      <c r="D81" t="s">
+        <v>260</v>
+      </c>
+      <c r="E81" t="s">
+        <v>135</v>
+      </c>
+      <c r="F81">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>250</v>
+      </c>
+      <c r="B82" t="s">
+        <v>251</v>
+      </c>
+      <c r="C82" t="s">
+        <v>378</v>
+      </c>
+      <c r="D82" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" t="s">
+        <v>135</v>
+      </c>
+      <c r="F82">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>252</v>
+      </c>
+      <c r="B83" t="s">
+        <v>253</v>
+      </c>
+      <c r="C83" t="s">
+        <v>379</v>
+      </c>
+      <c r="D83" t="s">
+        <v>262</v>
+      </c>
+      <c r="E83" t="s">
+        <v>135</v>
+      </c>
+      <c r="F83">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" t="s">
+        <v>255</v>
+      </c>
+      <c r="C84" t="s">
+        <v>343</v>
+      </c>
+      <c r="D84" t="s">
+        <v>263</v>
+      </c>
+      <c r="E84" t="s">
+        <v>135</v>
+      </c>
+      <c r="F84">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>256</v>
+      </c>
+      <c r="B85" t="s">
+        <v>257</v>
+      </c>
+      <c r="C85" t="s">
+        <v>380</v>
+      </c>
+      <c r="D85" t="s">
+        <v>264</v>
+      </c>
+      <c r="E85" t="s">
+        <v>135</v>
+      </c>
+      <c r="F85">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>258</v>
+      </c>
+      <c r="B86" t="s">
+        <v>259</v>
+      </c>
+      <c r="C86" t="s">
+        <v>381</v>
+      </c>
+      <c r="D86" t="s">
+        <v>265</v>
+      </c>
+      <c r="E86" t="s">
+        <v>135</v>
+      </c>
+      <c r="F86">
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B7AC9-630E-44A9-B0B1-248004C38CEC}">
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:D66" si="0">UPPER(IFERROR(LEFT(B3,FIND(" ",B3)),B3))</f>
+        <f t="shared" ref="C3:C66" si="0">UPPER(IFERROR(LEFT(B3,FIND(" ",B3)),B3))</f>
         <v>CLS</v>
       </c>
       <c r="D3" t="s">
@@ -3474,7 +5226,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
refractor instruction parsing and implement disassembly
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\chip16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B5B0B0-D2AA-4CCC-AAD9-E52C10523843}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857801FD-4E8F-4297-AABA-C194D6C950CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{46DFD0A6-98B0-40CA-87AE-5F9AE7027D73}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="411">
   <si>
     <t>00 00 00 00</t>
   </si>
@@ -838,9 +838,6 @@
     <t>SPR</t>
   </si>
   <si>
-    <t>DRW1</t>
-  </si>
-  <si>
     <t>RND</t>
   </si>
   <si>
@@ -907,18 +904,9 @@
     <t>DIVI</t>
   </si>
   <si>
-    <t>DRW0</t>
-  </si>
-  <si>
     <t>FLIP0</t>
   </si>
   <si>
-    <t>JMP1</t>
-  </si>
-  <si>
-    <t>CALL1</t>
-  </si>
-  <si>
     <t>FLIP1</t>
   </si>
   <si>
@@ -928,144 +916,24 @@
     <t>FLIP3</t>
   </si>
   <si>
-    <t>JMP0</t>
-  </si>
-  <si>
-    <t>CALL0</t>
-  </si>
-  <si>
-    <t>LDM0</t>
-  </si>
-  <si>
-    <t>STM0</t>
-  </si>
-  <si>
-    <t>ADD0</t>
-  </si>
-  <si>
-    <t>LDI0</t>
-  </si>
-  <si>
-    <t>LDI1</t>
-  </si>
-  <si>
-    <t>STM1</t>
-  </si>
-  <si>
-    <t>ADD1</t>
-  </si>
-  <si>
-    <t>LDM1</t>
-  </si>
-  <si>
-    <t>SUB0</t>
-  </si>
-  <si>
-    <t>AND0</t>
-  </si>
-  <si>
-    <t>OR0</t>
-  </si>
-  <si>
-    <t>XOR0</t>
-  </si>
-  <si>
-    <t>MUL0</t>
-  </si>
-  <si>
-    <t>DIV0</t>
-  </si>
-  <si>
-    <t>SUB1</t>
-  </si>
-  <si>
-    <t>AND1</t>
-  </si>
-  <si>
-    <t>OR1</t>
-  </si>
-  <si>
-    <t>XOR1</t>
-  </si>
-  <si>
-    <t>MUL1</t>
-  </si>
-  <si>
-    <t>DIV1</t>
-  </si>
-  <si>
-    <t>MOD0</t>
-  </si>
-  <si>
     <t>MODI</t>
   </si>
   <si>
-    <t>MOD1</t>
-  </si>
-  <si>
     <t>REMI</t>
   </si>
   <si>
-    <t>REM0</t>
-  </si>
-  <si>
-    <t>REM1</t>
-  </si>
-  <si>
-    <t>SHL0</t>
-  </si>
-  <si>
-    <t>SHR1</t>
-  </si>
-  <si>
-    <t>SHR0</t>
-  </si>
-  <si>
-    <t>SAL0</t>
-  </si>
-  <si>
-    <t>SAR0</t>
-  </si>
-  <si>
-    <t>SHL1</t>
-  </si>
-  <si>
-    <t>SAL1</t>
-  </si>
-  <si>
-    <t>SAR1</t>
-  </si>
-  <si>
     <t>PUSH</t>
   </si>
   <si>
     <t>POP</t>
   </si>
   <si>
-    <t>PAL0</t>
-  </si>
-  <si>
-    <t>PAL1</t>
-  </si>
-  <si>
     <t>NOTI</t>
   </si>
   <si>
-    <t>NOT0</t>
-  </si>
-  <si>
-    <t>NOT1</t>
-  </si>
-  <si>
     <t>NEGI</t>
   </si>
   <si>
-    <t>NEG0</t>
-  </si>
-  <si>
-    <t>NEG1</t>
-  </si>
-  <si>
     <t>DRWI</t>
   </si>
   <si>
@@ -1190,6 +1058,207 @@
   </si>
   <si>
     <t>SARR</t>
+  </si>
+  <si>
+    <t>LDR_I</t>
+  </si>
+  <si>
+    <t>LDS_I</t>
+  </si>
+  <si>
+    <t>ADD_R2</t>
+  </si>
+  <si>
+    <t>ADD_R3</t>
+  </si>
+  <si>
+    <t>ADD_I</t>
+  </si>
+  <si>
+    <t>SUB_I</t>
+  </si>
+  <si>
+    <t>SUB_R2</t>
+  </si>
+  <si>
+    <t>SUB_R3</t>
+  </si>
+  <si>
+    <t>STM_I</t>
+  </si>
+  <si>
+    <t>STM_R</t>
+  </si>
+  <si>
+    <t>LDM_R</t>
+  </si>
+  <si>
+    <t>LDM_I</t>
+  </si>
+  <si>
+    <t>CALL_I</t>
+  </si>
+  <si>
+    <t>CALL_R</t>
+  </si>
+  <si>
+    <t>JMP_I</t>
+  </si>
+  <si>
+    <t>JMP_R</t>
+  </si>
+  <si>
+    <t>FLIP</t>
+  </si>
+  <si>
+    <t>DRW_I</t>
+  </si>
+  <si>
+    <t>DRW_R</t>
+  </si>
+  <si>
+    <t>CMP_I</t>
+  </si>
+  <si>
+    <t>CMP_R</t>
+  </si>
+  <si>
+    <t>AND_I</t>
+  </si>
+  <si>
+    <t>AND_R2</t>
+  </si>
+  <si>
+    <t>AND_R3</t>
+  </si>
+  <si>
+    <t>TST_I</t>
+  </si>
+  <si>
+    <t>TST_R</t>
+  </si>
+  <si>
+    <t>OR_I</t>
+  </si>
+  <si>
+    <t>OR_R2</t>
+  </si>
+  <si>
+    <t>OR_R3</t>
+  </si>
+  <si>
+    <t>XOR_I</t>
+  </si>
+  <si>
+    <t>MUL_I</t>
+  </si>
+  <si>
+    <t>D_IV_I</t>
+  </si>
+  <si>
+    <t>MOD_I</t>
+  </si>
+  <si>
+    <t>REM_I</t>
+  </si>
+  <si>
+    <t>XOR_R2</t>
+  </si>
+  <si>
+    <t>MUL_R2</t>
+  </si>
+  <si>
+    <t>DIV_R2</t>
+  </si>
+  <si>
+    <t>MOD_R2</t>
+  </si>
+  <si>
+    <t>REM_R2</t>
+  </si>
+  <si>
+    <t>XOR_R3</t>
+  </si>
+  <si>
+    <t>MUL_R3</t>
+  </si>
+  <si>
+    <t>DIV_R3</t>
+  </si>
+  <si>
+    <t>MOD_R3</t>
+  </si>
+  <si>
+    <t>REM_R3</t>
+  </si>
+  <si>
+    <t>SHL_N</t>
+  </si>
+  <si>
+    <t>SHR_N</t>
+  </si>
+  <si>
+    <t>SAL_N</t>
+  </si>
+  <si>
+    <t>SAR_N</t>
+  </si>
+  <si>
+    <t>SHL_R</t>
+  </si>
+  <si>
+    <t>SHR_R</t>
+  </si>
+  <si>
+    <t>SAL_R</t>
+  </si>
+  <si>
+    <t>SAR_R</t>
+  </si>
+  <si>
+    <t>PAL_I</t>
+  </si>
+  <si>
+    <t>PAL_R</t>
+  </si>
+  <si>
+    <t>NOT_I</t>
+  </si>
+  <si>
+    <t>NOT_R</t>
+  </si>
+  <si>
+    <t>NOT_R2</t>
+  </si>
+  <si>
+    <t>NEG_I</t>
+  </si>
+  <si>
+    <t>NEG_R</t>
+  </si>
+  <si>
+    <t>NEG_R2</t>
+  </si>
+  <si>
+    <t>no_underscore</t>
+  </si>
+  <si>
+    <t>CMPR</t>
+  </si>
+  <si>
+    <t>TSTR</t>
+  </si>
+  <si>
+    <t>SALN</t>
+  </si>
+  <si>
+    <t>SALR</t>
+  </si>
+  <si>
+    <t>NOTR</t>
+  </si>
+  <si>
+    <t>NEGR</t>
   </si>
 </sst>
 </file>
@@ -1239,16 +1308,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1718,7 +1829,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>302</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1738,7 +1849,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>347</v>
+        <v>303</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -1758,7 +1869,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -1775,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D10" t="s">
         <v>47</v>
@@ -1792,7 +1903,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
@@ -1809,7 +1920,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
@@ -1826,7 +1937,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
         <v>50</v>
@@ -1860,7 +1971,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -1877,7 +1988,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1894,7 +2005,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -1911,7 +2022,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
@@ -1928,7 +2039,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -1945,7 +2056,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>348</v>
+        <v>304</v>
       </c>
       <c r="D20" t="s">
         <v>79</v>
@@ -1962,7 +2073,7 @@
         <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
@@ -1979,7 +2090,7 @@
         <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22" t="s">
         <v>80</v>
@@ -1996,7 +2107,7 @@
         <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D23" t="s">
         <v>81</v>
@@ -2013,7 +2124,7 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>349</v>
+        <v>305</v>
       </c>
       <c r="D24" t="s">
         <v>82</v>
@@ -2047,7 +2158,7 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>350</v>
+        <v>306</v>
       </c>
       <c r="D26" t="s">
         <v>84</v>
@@ -2064,7 +2175,7 @@
         <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D27" t="s">
         <v>85</v>
@@ -2081,7 +2192,7 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>351</v>
+        <v>307</v>
       </c>
       <c r="D28" t="s">
         <v>86</v>
@@ -2098,7 +2209,7 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>352</v>
+        <v>308</v>
       </c>
       <c r="D29" t="s">
         <v>97</v>
@@ -2115,7 +2226,7 @@
         <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>353</v>
+        <v>309</v>
       </c>
       <c r="D30" t="s">
         <v>98</v>
@@ -2132,7 +2243,7 @@
         <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>354</v>
+        <v>310</v>
       </c>
       <c r="D31" t="s">
         <v>99</v>
@@ -2149,7 +2260,7 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>355</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
         <v>100</v>
@@ -2166,7 +2277,7 @@
         <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D33" t="s">
         <v>101</v>
@@ -2183,7 +2294,7 @@
         <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>356</v>
+        <v>312</v>
       </c>
       <c r="D34" t="s">
         <v>106</v>
@@ -2200,7 +2311,7 @@
         <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>357</v>
+        <v>313</v>
       </c>
       <c r="D35" t="s">
         <v>107</v>
@@ -2217,7 +2328,7 @@
         <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D36" t="s">
         <v>115</v>
@@ -2237,7 +2348,7 @@
         <v>112</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>358</v>
+        <v>314</v>
       </c>
       <c r="D37" t="s">
         <v>116</v>
@@ -2257,7 +2368,7 @@
         <v>114</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="D38" t="s">
         <v>117</v>
@@ -2277,7 +2388,7 @@
         <v>119</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D39" t="s">
         <v>128</v>
@@ -2297,7 +2408,7 @@
         <v>121</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>360</v>
+        <v>316</v>
       </c>
       <c r="D40" t="s">
         <v>129</v>
@@ -2317,7 +2428,7 @@
         <v>123</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>361</v>
+        <v>317</v>
       </c>
       <c r="D41" t="s">
         <v>130</v>
@@ -2337,7 +2448,7 @@
         <v>125</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D42" t="s">
         <v>131</v>
@@ -2357,7 +2468,7 @@
         <v>127</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D43" t="s">
         <v>132</v>
@@ -2377,7 +2488,7 @@
         <v>134</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D44" t="s">
         <v>144</v>
@@ -2397,7 +2508,7 @@
         <v>137</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>362</v>
+        <v>318</v>
       </c>
       <c r="D45" t="s">
         <v>145</v>
@@ -2417,7 +2528,7 @@
         <v>139</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>363</v>
+        <v>319</v>
       </c>
       <c r="D46" t="s">
         <v>146</v>
@@ -2437,7 +2548,7 @@
         <v>141</v>
       </c>
       <c r="C47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D47" t="s">
         <v>147</v>
@@ -2457,7 +2568,7 @@
         <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D48" t="s">
         <v>148</v>
@@ -2477,7 +2588,7 @@
         <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D49" t="s">
         <v>155</v>
@@ -2497,7 +2608,7 @@
         <v>152</v>
       </c>
       <c r="C50" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
       <c r="D50" t="s">
         <v>156</v>
@@ -2517,7 +2628,7 @@
         <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="D51" t="s">
         <v>157</v>
@@ -2537,7 +2648,7 @@
         <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D52" t="s">
         <v>164</v>
@@ -2557,7 +2668,7 @@
         <v>161</v>
       </c>
       <c r="C53" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="D53" t="s">
         <v>165</v>
@@ -2577,7 +2688,7 @@
         <v>163</v>
       </c>
       <c r="C54" t="s">
-        <v>367</v>
+        <v>323</v>
       </c>
       <c r="D54" t="s">
         <v>166</v>
@@ -2597,7 +2708,7 @@
         <v>168</v>
       </c>
       <c r="C55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D55" t="s">
         <v>174</v>
@@ -2617,7 +2728,7 @@
         <v>171</v>
       </c>
       <c r="C56" t="s">
-        <v>368</v>
+        <v>324</v>
       </c>
       <c r="D56" t="s">
         <v>175</v>
@@ -2637,7 +2748,7 @@
         <v>173</v>
       </c>
       <c r="C57" t="s">
-        <v>369</v>
+        <v>325</v>
       </c>
       <c r="D57" t="s">
         <v>176</v>
@@ -2657,7 +2768,7 @@
         <v>178</v>
       </c>
       <c r="C58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D58" t="s">
         <v>195</v>
@@ -2677,7 +2788,7 @@
         <v>180</v>
       </c>
       <c r="C59" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="D59" t="s">
         <v>196</v>
@@ -2697,7 +2808,7 @@
         <v>182</v>
       </c>
       <c r="C60" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="D60" t="s">
         <v>197</v>
@@ -2717,7 +2828,7 @@
         <v>184</v>
       </c>
       <c r="C61" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="D61" t="s">
         <v>198</v>
@@ -2737,7 +2848,7 @@
         <v>186</v>
       </c>
       <c r="C62" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="D62" t="s">
         <v>199</v>
@@ -2757,7 +2868,7 @@
         <v>188</v>
       </c>
       <c r="C63" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="D63" t="s">
         <v>200</v>
@@ -2777,7 +2888,7 @@
         <v>190</v>
       </c>
       <c r="C64" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
       <c r="D64" t="s">
         <v>201</v>
@@ -2797,7 +2908,7 @@
         <v>192</v>
       </c>
       <c r="C65" t="s">
-        <v>374</v>
+        <v>330</v>
       </c>
       <c r="D65" t="s">
         <v>202</v>
@@ -2817,7 +2928,7 @@
         <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>375</v>
+        <v>331</v>
       </c>
       <c r="D66" t="s">
         <v>203</v>
@@ -2837,7 +2948,7 @@
         <v>205</v>
       </c>
       <c r="C67" t="s">
-        <v>382</v>
+        <v>338</v>
       </c>
       <c r="D67" t="s">
         <v>218</v>
@@ -2857,7 +2968,7 @@
         <v>207</v>
       </c>
       <c r="C68" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="D68" t="s">
         <v>219</v>
@@ -2877,7 +2988,7 @@
         <v>210</v>
       </c>
       <c r="C69" t="s">
-        <v>384</v>
+        <v>340</v>
       </c>
       <c r="D69" t="s">
         <v>220</v>
@@ -2897,7 +3008,7 @@
         <v>212</v>
       </c>
       <c r="C70" t="s">
-        <v>385</v>
+        <v>341</v>
       </c>
       <c r="D70" t="s">
         <v>221</v>
@@ -2917,7 +3028,7 @@
         <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="D71" t="s">
         <v>222</v>
@@ -2937,7 +3048,7 @@
         <v>217</v>
       </c>
       <c r="C72" t="s">
-        <v>387</v>
+        <v>343</v>
       </c>
       <c r="D72" t="s">
         <v>223</v>
@@ -2957,7 +3068,7 @@
         <v>225</v>
       </c>
       <c r="C73" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="D73" t="s">
         <v>236</v>
@@ -2974,7 +3085,7 @@
         <v>227</v>
       </c>
       <c r="C74" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="D74" t="s">
         <v>237</v>
@@ -3059,7 +3170,7 @@
         <v>243</v>
       </c>
       <c r="C79" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="D79" t="s">
         <v>246</v>
@@ -3076,7 +3187,7 @@
         <v>245</v>
       </c>
       <c r="C80" t="s">
-        <v>377</v>
+        <v>333</v>
       </c>
       <c r="D80" t="s">
         <v>247</v>
@@ -3093,7 +3204,7 @@
         <v>249</v>
       </c>
       <c r="C81" t="s">
-        <v>340</v>
+        <v>300</v>
       </c>
       <c r="D81" t="s">
         <v>260</v>
@@ -3113,7 +3224,7 @@
         <v>251</v>
       </c>
       <c r="C82" t="s">
-        <v>378</v>
+        <v>334</v>
       </c>
       <c r="D82" t="s">
         <v>261</v>
@@ -3133,7 +3244,7 @@
         <v>253</v>
       </c>
       <c r="C83" t="s">
-        <v>379</v>
+        <v>335</v>
       </c>
       <c r="D83" t="s">
         <v>262</v>
@@ -3153,7 +3264,7 @@
         <v>255</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="D84" t="s">
         <v>263</v>
@@ -3173,7 +3284,7 @@
         <v>257</v>
       </c>
       <c r="C85" t="s">
-        <v>380</v>
+        <v>336</v>
       </c>
       <c r="D85" t="s">
         <v>264</v>
@@ -3193,7 +3304,7 @@
         <v>259</v>
       </c>
       <c r="C86" t="s">
-        <v>381</v>
+        <v>337</v>
       </c>
       <c r="D86" t="s">
         <v>265</v>
@@ -3207,7 +3318,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3216,10 +3327,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B7AC9-630E-44A9-B0B1-248004C38CEC}">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3228,12 +3339,13 @@
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -3247,16 +3359,19 @@
         <v>267</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3267,17 +3382,20 @@
         <f>UPPER(IFERROR(LEFT(B2,FIND(" ",B2)),B2))</f>
         <v>NOP</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3288,17 +3406,20 @@
         <f t="shared" ref="C3:C66" si="0">UPPER(IFERROR(LEFT(B3,FIND(" ",B3)),B3))</f>
         <v>CLS</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="G3">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3309,17 +3430,20 @@
         <f t="shared" si="0"/>
         <v>VBLNK</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>41</v>
       </c>
-      <c r="G4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3330,17 +3454,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">BGC </v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="G5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3351,17 +3478,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SPR </v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" t="s">
         <v>43</v>
       </c>
-      <c r="G6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3372,20 +3502,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">DRW </v>
       </c>
-      <c r="D7" t="s">
-        <v>293</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="G7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3396,20 +3529,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">DRW </v>
       </c>
-      <c r="D8" t="s">
-        <v>270</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="G8">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3420,17 +3556,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">RND </v>
       </c>
-      <c r="D9" t="s">
-        <v>271</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F9" t="s">
         <v>46</v>
       </c>
-      <c r="G9">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3441,17 +3580,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D10" t="s">
-        <v>294</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="G10">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3462,17 +3604,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D11" t="s">
-        <v>297</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F11" t="s">
         <v>48</v>
       </c>
-      <c r="G11">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -3483,17 +3628,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D12" t="s">
-        <v>298</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="G12">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3504,17 +3652,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D13" t="s">
-        <v>299</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="F13" t="s">
         <v>50</v>
       </c>
-      <c r="G13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3525,17 +3676,20 @@
         <f t="shared" si="0"/>
         <v>SND0</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
         <v>28</v>
       </c>
-      <c r="G14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3546,17 +3700,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SND1 </v>
       </c>
-      <c r="D15" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" t="s">
         <v>51</v>
       </c>
-      <c r="G15">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3567,17 +3724,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SND2 </v>
       </c>
-      <c r="D16" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F16" t="s">
         <v>52</v>
       </c>
-      <c r="G16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3588,17 +3748,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SND3 </v>
       </c>
-      <c r="D17" t="s">
-        <v>274</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="G17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3609,17 +3772,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SNP </v>
       </c>
-      <c r="D18" t="s">
-        <v>275</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" t="s">
         <v>54</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3630,17 +3796,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SNG </v>
       </c>
-      <c r="D19" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F19" t="s">
         <v>39</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -3651,17 +3820,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">JMP </v>
       </c>
-      <c r="D20" t="s">
-        <v>300</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F20" t="s">
         <v>79</v>
       </c>
-      <c r="G20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -3672,17 +3844,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">JMC </v>
       </c>
-      <c r="D21" t="s">
-        <v>277</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F21" t="s">
         <v>64</v>
       </c>
-      <c r="G21">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3693,17 +3868,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">JX </v>
       </c>
-      <c r="D22" t="s">
-        <v>278</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" t="s">
         <v>80</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3714,17 +3892,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">JME </v>
       </c>
-      <c r="D23" t="s">
-        <v>279</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F23" t="s">
         <v>81</v>
       </c>
-      <c r="G23">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -3735,17 +3916,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">CALL </v>
       </c>
-      <c r="D24" t="s">
-        <v>301</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F24" t="s">
         <v>82</v>
       </c>
-      <c r="G24">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3756,17 +3940,20 @@
         <f t="shared" si="0"/>
         <v>RET</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
         <v>83</v>
       </c>
-      <c r="G25">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -3777,17 +3964,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">JMP </v>
       </c>
-      <c r="D26" t="s">
-        <v>295</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F26" t="s">
         <v>84</v>
       </c>
-      <c r="G26">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -3798,17 +3988,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">CX </v>
       </c>
-      <c r="D27" t="s">
-        <v>280</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F27" t="s">
         <v>85</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -3819,17 +4012,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">CALL </v>
       </c>
-      <c r="D28" t="s">
-        <v>296</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F28" t="s">
         <v>86</v>
       </c>
-      <c r="G28">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -3840,17 +4036,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">LDI </v>
       </c>
-      <c r="D29" t="s">
-        <v>305</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F29" t="s">
         <v>97</v>
       </c>
-      <c r="G29">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -3861,17 +4060,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">LDI </v>
       </c>
-      <c r="D30" t="s">
-        <v>306</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F30" t="s">
         <v>98</v>
       </c>
-      <c r="G30">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -3882,17 +4084,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">LDM </v>
       </c>
-      <c r="D31" t="s">
-        <v>302</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F31" t="s">
         <v>99</v>
       </c>
-      <c r="G31">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -3903,17 +4108,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">LDM </v>
       </c>
-      <c r="D32" t="s">
-        <v>309</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F32" t="s">
         <v>100</v>
       </c>
-      <c r="G32">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -3924,17 +4132,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MOV </v>
       </c>
-      <c r="D33" t="s">
-        <v>281</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D33" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F33" t="s">
         <v>101</v>
       </c>
-      <c r="G33">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -3945,17 +4156,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">STM </v>
       </c>
-      <c r="D34" t="s">
-        <v>303</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D34" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="F34" t="s">
         <v>106</v>
       </c>
-      <c r="G34">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -3966,17 +4180,20 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">STM </v>
       </c>
-      <c r="D35" t="s">
-        <v>307</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F35" t="s">
         <v>107</v>
       </c>
-      <c r="G35">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -3987,20 +4204,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">ADDI </v>
       </c>
-      <c r="D36" t="s">
-        <v>282</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F36" t="s">
         <v>115</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>110</v>
       </c>
-      <c r="G36">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -4011,20 +4231,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">ADD </v>
       </c>
-      <c r="D37" t="s">
-        <v>304</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D37" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F37" t="s">
         <v>116</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>110</v>
       </c>
-      <c r="G37">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -4035,20 +4258,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">ADD </v>
       </c>
-      <c r="D38" t="s">
-        <v>308</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F38" t="s">
         <v>117</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>110</v>
       </c>
-      <c r="G38">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -4059,20 +4285,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SUBI </v>
       </c>
-      <c r="D39" t="s">
-        <v>283</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F39" t="s">
         <v>128</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>110</v>
       </c>
-      <c r="G39">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -4083,20 +4312,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SUB </v>
       </c>
-      <c r="D40" t="s">
-        <v>310</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D40" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F40" t="s">
         <v>129</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>110</v>
       </c>
-      <c r="G40">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -4107,20 +4339,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">SUB </v>
       </c>
-      <c r="D41" t="s">
-        <v>316</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F41" t="s">
         <v>130</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>110</v>
       </c>
-      <c r="G41">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -4131,20 +4366,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">CMPI </v>
       </c>
-      <c r="D42" t="s">
-        <v>284</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D42" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F42" t="s">
         <v>131</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>110</v>
       </c>
-      <c r="G42">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -4155,20 +4393,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">CMP </v>
       </c>
-      <c r="D43" t="s">
-        <v>285</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F43" t="s">
         <v>132</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>110</v>
       </c>
-      <c r="G43">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -4179,20 +4420,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">ANDI </v>
       </c>
-      <c r="D44" t="s">
-        <v>286</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D44" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F44" t="s">
         <v>144</v>
       </c>
-      <c r="F44" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -4203,20 +4447,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">AND </v>
       </c>
-      <c r="D45" t="s">
-        <v>311</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D45" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F45" t="s">
         <v>145</v>
       </c>
-      <c r="F45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>135</v>
+      </c>
+      <c r="H45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>138</v>
       </c>
@@ -4227,20 +4474,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">AND </v>
       </c>
-      <c r="D46" t="s">
-        <v>317</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D46" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F46" t="s">
         <v>146</v>
       </c>
-      <c r="F46" t="s">
-        <v>135</v>
-      </c>
-      <c r="G46">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -4251,20 +4501,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">TSTI </v>
       </c>
-      <c r="D47" t="s">
-        <v>287</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F47" t="s">
         <v>147</v>
       </c>
-      <c r="F47" t="s">
-        <v>135</v>
-      </c>
-      <c r="G47">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>135</v>
+      </c>
+      <c r="H47">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -4275,20 +4528,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">TST </v>
       </c>
-      <c r="D48" t="s">
-        <v>288</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D48" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="F48" t="s">
         <v>148</v>
       </c>
-      <c r="F48" t="s">
-        <v>135</v>
-      </c>
-      <c r="G48">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>135</v>
+      </c>
+      <c r="H48">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -4299,20 +4555,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">ORI </v>
       </c>
-      <c r="D49" t="s">
-        <v>289</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F49" t="s">
         <v>155</v>
       </c>
-      <c r="F49" t="s">
-        <v>135</v>
-      </c>
-      <c r="G49">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>151</v>
       </c>
@@ -4323,20 +4582,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">OR </v>
       </c>
-      <c r="D50" t="s">
-        <v>312</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D50" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F50" t="s">
         <v>156</v>
       </c>
-      <c r="F50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G50">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>135</v>
+      </c>
+      <c r="H50">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>153</v>
       </c>
@@ -4347,20 +4609,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">OR </v>
       </c>
-      <c r="D51" t="s">
-        <v>318</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D51" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F51" t="s">
         <v>157</v>
       </c>
-      <c r="F51" t="s">
-        <v>135</v>
-      </c>
-      <c r="G51">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>135</v>
+      </c>
+      <c r="H51">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>158</v>
       </c>
@@ -4371,20 +4636,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">XORI </v>
       </c>
-      <c r="D52" t="s">
-        <v>290</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F52" t="s">
         <v>164</v>
       </c>
-      <c r="F52" t="s">
-        <v>135</v>
-      </c>
-      <c r="G52">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>160</v>
       </c>
@@ -4395,20 +4663,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">XOR </v>
       </c>
-      <c r="D53" t="s">
-        <v>313</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F53" t="s">
         <v>165</v>
       </c>
-      <c r="F53" t="s">
-        <v>135</v>
-      </c>
-      <c r="G53">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>135</v>
+      </c>
+      <c r="H53">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>162</v>
       </c>
@@ -4419,20 +4690,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">XOR </v>
       </c>
-      <c r="D54" t="s">
-        <v>319</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D54" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F54" t="s">
         <v>166</v>
       </c>
-      <c r="F54" t="s">
-        <v>135</v>
-      </c>
-      <c r="G54">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>135</v>
+      </c>
+      <c r="H54">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -4443,20 +4717,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MULI </v>
       </c>
-      <c r="D55" t="s">
-        <v>291</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D55" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F55" t="s">
         <v>174</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>169</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>170</v>
       </c>
@@ -4467,20 +4744,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MUL </v>
       </c>
-      <c r="D56" t="s">
-        <v>314</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D56" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F56" t="s">
         <v>175</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>169</v>
       </c>
-      <c r="G56">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -4491,20 +4771,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MUL </v>
       </c>
-      <c r="D57" t="s">
-        <v>320</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="D57" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F57" t="s">
         <v>176</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>169</v>
       </c>
-      <c r="G57">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>177</v>
       </c>
@@ -4515,20 +4798,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">DIVI </v>
       </c>
-      <c r="D58" t="s">
-        <v>292</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D58" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F58" t="s">
         <v>195</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>169</v>
       </c>
-      <c r="G58">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -4539,20 +4825,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">DIV </v>
       </c>
-      <c r="D59" t="s">
-        <v>315</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D59" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F59" t="s">
         <v>196</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>169</v>
       </c>
-      <c r="G59">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>181</v>
       </c>
@@ -4563,20 +4852,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">DIV </v>
       </c>
-      <c r="D60" t="s">
-        <v>321</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D60" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F60" t="s">
         <v>197</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>169</v>
       </c>
-      <c r="G60">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>183</v>
       </c>
@@ -4587,20 +4879,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MODI </v>
       </c>
-      <c r="D61" t="s">
-        <v>323</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D61" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F61" t="s">
         <v>198</v>
       </c>
-      <c r="F61" t="s">
-        <v>135</v>
-      </c>
-      <c r="G61">
+      <c r="G61" t="s">
+        <v>135</v>
+      </c>
+      <c r="H61">
         <v>1.3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -4611,20 +4906,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MOD </v>
       </c>
-      <c r="D62" t="s">
-        <v>322</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="D62" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F62" t="s">
         <v>199</v>
       </c>
-      <c r="F62" t="s">
-        <v>135</v>
-      </c>
-      <c r="G62">
+      <c r="G62" t="s">
+        <v>135</v>
+      </c>
+      <c r="H62">
         <v>1.3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -4635,20 +4933,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">MOD </v>
       </c>
-      <c r="D63" t="s">
-        <v>324</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D63" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F63" t="s">
         <v>200</v>
       </c>
-      <c r="F63" t="s">
-        <v>135</v>
-      </c>
-      <c r="G63">
+      <c r="G63" t="s">
+        <v>135</v>
+      </c>
+      <c r="H63">
         <v>1.3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -4659,20 +4960,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">REMI </v>
       </c>
-      <c r="D64" t="s">
-        <v>325</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="D64" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F64" t="s">
         <v>201</v>
       </c>
-      <c r="F64" t="s">
-        <v>135</v>
-      </c>
-      <c r="G64">
+      <c r="G64" t="s">
+        <v>135</v>
+      </c>
+      <c r="H64">
         <v>1.3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -4683,20 +4987,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">REM </v>
       </c>
-      <c r="D65" t="s">
-        <v>326</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="D65" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F65" t="s">
         <v>202</v>
       </c>
-      <c r="F65" t="s">
-        <v>135</v>
-      </c>
-      <c r="G65">
+      <c r="G65" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65">
         <v>1.3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -4707,20 +5014,23 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">REM </v>
       </c>
-      <c r="D66" t="s">
-        <v>327</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="D66" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F66" t="s">
         <v>203</v>
       </c>
-      <c r="F66" t="s">
-        <v>135</v>
-      </c>
-      <c r="G66">
+      <c r="G66" t="s">
+        <v>135</v>
+      </c>
+      <c r="H66">
         <v>1.3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>204</v>
       </c>
@@ -4731,20 +5041,23 @@
         <f t="shared" ref="C67:C88" si="1">UPPER(IFERROR(LEFT(B67,FIND(" ",B67)),B67))</f>
         <v xml:space="preserve">SHL </v>
       </c>
-      <c r="D67" t="s">
-        <v>328</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="D67" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F67" t="s">
         <v>218</v>
       </c>
-      <c r="F67" t="s">
-        <v>135</v>
-      </c>
-      <c r="G67">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>135</v>
+      </c>
+      <c r="H67">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>206</v>
       </c>
@@ -4755,20 +5068,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SHR </v>
       </c>
-      <c r="D68" t="s">
-        <v>330</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D68" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F68" t="s">
         <v>219</v>
       </c>
-      <c r="F68" t="s">
-        <v>135</v>
-      </c>
-      <c r="G68">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>135</v>
+      </c>
+      <c r="H68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>204</v>
       </c>
@@ -4779,20 +5095,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SAL </v>
       </c>
-      <c r="D69" t="s">
-        <v>331</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="D69" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F69" t="s">
         <v>218</v>
       </c>
-      <c r="F69" t="s">
-        <v>135</v>
-      </c>
-      <c r="G69">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>135</v>
+      </c>
+      <c r="H69">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>209</v>
       </c>
@@ -4803,20 +5122,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SAR </v>
       </c>
-      <c r="D70" t="s">
-        <v>332</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="D70" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F70" t="s">
         <v>220</v>
       </c>
-      <c r="F70" t="s">
-        <v>135</v>
-      </c>
-      <c r="G70">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>135</v>
+      </c>
+      <c r="H70">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>211</v>
       </c>
@@ -4827,20 +5149,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SHL </v>
       </c>
-      <c r="D71" t="s">
-        <v>333</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D71" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F71" t="s">
         <v>221</v>
       </c>
-      <c r="F71" t="s">
-        <v>135</v>
-      </c>
-      <c r="G71">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>135</v>
+      </c>
+      <c r="H71">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -4851,20 +5176,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SHR </v>
       </c>
-      <c r="D72" t="s">
-        <v>329</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="D72" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F72" t="s">
         <v>222</v>
       </c>
-      <c r="F72" t="s">
-        <v>135</v>
-      </c>
-      <c r="G72">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>135</v>
+      </c>
+      <c r="H72">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>211</v>
       </c>
@@ -4875,20 +5203,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SAL </v>
       </c>
-      <c r="D73" t="s">
-        <v>334</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="D73" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="F73" t="s">
         <v>221</v>
       </c>
-      <c r="F73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G73">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>135</v>
+      </c>
+      <c r="H73">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>216</v>
       </c>
@@ -4899,20 +5230,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">SAR </v>
       </c>
-      <c r="D74" t="s">
-        <v>335</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="D74" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F74" t="s">
         <v>223</v>
       </c>
-      <c r="F74" t="s">
-        <v>135</v>
-      </c>
-      <c r="G74">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>135</v>
+      </c>
+      <c r="H74">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>224</v>
       </c>
@@ -4923,17 +5257,20 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">PUSH </v>
       </c>
-      <c r="D75" t="s">
-        <v>336</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="D75" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F75" t="s">
         <v>236</v>
       </c>
-      <c r="G75">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>226</v>
       </c>
@@ -4944,17 +5281,20 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">POP </v>
       </c>
-      <c r="D76" t="s">
-        <v>337</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="D76" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F76" t="s">
         <v>237</v>
       </c>
-      <c r="G76">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -4965,17 +5305,20 @@
         <f t="shared" si="1"/>
         <v>PUSHALL</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F77" t="s">
         <v>238</v>
       </c>
-      <c r="G77">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>230</v>
       </c>
@@ -4986,17 +5329,20 @@
         <f t="shared" si="1"/>
         <v>POPALL</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F78" t="s">
         <v>239</v>
       </c>
-      <c r="G78">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>232</v>
       </c>
@@ -5007,17 +5353,20 @@
         <f t="shared" si="1"/>
         <v>PUSHF</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F79" t="s">
         <v>240</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>234</v>
       </c>
@@ -5028,17 +5377,20 @@
         <f t="shared" si="1"/>
         <v>POPF</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F80" t="s">
         <v>241</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -5049,17 +5401,20 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">PAL </v>
       </c>
-      <c r="D81" t="s">
-        <v>338</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="D81" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F81" t="s">
         <v>246</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>244</v>
       </c>
@@ -5070,17 +5425,20 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">PAL </v>
       </c>
-      <c r="D82" t="s">
-        <v>339</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D82" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F82" t="s">
         <v>247</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>248</v>
       </c>
@@ -5091,20 +5449,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NOTI </v>
       </c>
-      <c r="D83" t="s">
-        <v>340</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D83" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F83" t="s">
         <v>260</v>
       </c>
-      <c r="F83" t="s">
-        <v>135</v>
-      </c>
-      <c r="G83">
+      <c r="G83" t="s">
+        <v>135</v>
+      </c>
+      <c r="H83">
         <v>1.3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>250</v>
       </c>
@@ -5115,20 +5476,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NOT </v>
       </c>
-      <c r="D84" t="s">
-        <v>341</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D84" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F84" t="s">
         <v>261</v>
       </c>
-      <c r="F84" t="s">
-        <v>135</v>
-      </c>
-      <c r="G84">
+      <c r="G84" t="s">
+        <v>135</v>
+      </c>
+      <c r="H84">
         <v>1.3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>252</v>
       </c>
@@ -5139,20 +5503,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NOT </v>
       </c>
-      <c r="D85" t="s">
-        <v>342</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="D85" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F85" t="s">
         <v>262</v>
       </c>
-      <c r="F85" t="s">
-        <v>135</v>
-      </c>
-      <c r="G85">
+      <c r="G85" t="s">
+        <v>135</v>
+      </c>
+      <c r="H85">
         <v>1.3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>254</v>
       </c>
@@ -5163,20 +5530,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NEGI </v>
       </c>
-      <c r="D86" t="s">
-        <v>343</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="D86" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F86" t="s">
         <v>263</v>
       </c>
-      <c r="F86" t="s">
-        <v>135</v>
-      </c>
-      <c r="G86">
+      <c r="G86" t="s">
+        <v>135</v>
+      </c>
+      <c r="H86">
         <v>1.3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>256</v>
       </c>
@@ -5187,20 +5557,23 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NEG </v>
       </c>
-      <c r="D87" t="s">
-        <v>344</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="D87" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F87" t="s">
         <v>264</v>
       </c>
-      <c r="F87" t="s">
-        <v>135</v>
-      </c>
-      <c r="G87">
+      <c r="G87" t="s">
+        <v>135</v>
+      </c>
+      <c r="H87">
         <v>1.3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>258</v>
       </c>
@@ -5211,25 +5584,31 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">NEG </v>
       </c>
-      <c r="D88" t="s">
-        <v>345</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="D88" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F88" t="s">
         <v>265</v>
       </c>
-      <c r="F88" t="s">
-        <v>135</v>
-      </c>
-      <c r="G88">
+      <c r="G88" t="s">
+        <v>135</v>
+      </c>
+      <c r="H88">
         <v>1.3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
work on breaking instructions up into formats
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\chip16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857801FD-4E8F-4297-AABA-C194D6C950CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E7E90D-1F30-48B7-8F24-7626590B01AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{46DFD0A6-98B0-40CA-87AE-5F9AE7027D73}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
     <sheet name="instructions_old" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">instructions_old!$A$1:$I$88</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="423">
   <si>
     <t>00 00 00 00</t>
   </si>
@@ -1259,13 +1262,49 @@
   </si>
   <si>
     <t>NEGR</t>
+  </si>
+  <si>
+    <t>instruction_format</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>R_R_I</t>
+  </si>
+  <si>
+    <t>R_R_R</t>
+  </si>
+  <si>
+    <t>R_I</t>
+  </si>
+  <si>
+    <t>SP_I</t>
+  </si>
+  <si>
+    <t>R_R</t>
+  </si>
+  <si>
+    <t>R_N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1280,6 +1319,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1308,48 +1360,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3318,7 +3341,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3327,2287 +3350,2551 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B7AC9-630E-44A9-B0B1-248004C38CEC}">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="5" t="str">
         <f>UPPER(IFERROR(LEFT(B2,FIND(" ",B2)),B2))</f>
         <v>NOP</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="I2" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C66" si="0">UPPER(IFERROR(LEFT(B3,FIND(" ",B3)),B3))</f>
+      <c r="C3" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B3,FIND(" ",B3)),B3))</f>
         <v>CLS</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H3">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I3" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
+      <c r="C4" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B4,FIND(" ",B4)),B4))</f>
         <v>VBLNK</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I4" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
+      <c r="C5" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B5,FIND(" ",B5)),B5))</f>
         <v xml:space="preserve">BGC </v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="I5" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
+      <c r="C6" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B6,FIND(" ",B6)),B6))</f>
         <v xml:space="preserve">SPR </v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I6" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
+      <c r="C7" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B7,FIND(" ",B7)),B7))</f>
         <v xml:space="preserve">DRW </v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="I7" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
+      <c r="C8" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B8,FIND(" ",B8)),B8))</f>
         <v xml:space="preserve">DRW </v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H8">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I8" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
+      <c r="C9" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B9,FIND(" ",B9)),B9))</f>
         <v xml:space="preserve">RND </v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H9">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="I9" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
+      <c r="C10" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B10,FIND(" ",B10)),B10))</f>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H10">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I10" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
+      <c r="C11" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B11,FIND(" ",B11)),B11))</f>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H11">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="I11" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
+      <c r="C12" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B12,FIND(" ",B12)),B12))</f>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H12">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="I12" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
+      <c r="C13" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B13,FIND(" ",B13)),B13))</f>
         <v xml:space="preserve">FLIP </v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H13">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="I13" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
+      <c r="C14" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B14,FIND(" ",B14)),B14))</f>
         <v>SND0</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I14" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
+      <c r="C15" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B15,FIND(" ",B15)),B15))</f>
         <v xml:space="preserve">SND1 </v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H15">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I15" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
+      <c r="C16" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B16,FIND(" ",B16)),B16))</f>
         <v xml:space="preserve">SND2 </v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="I16" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
+      <c r="C17" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B17,FIND(" ",B17)),B17))</f>
         <v xml:space="preserve">SND3 </v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H17">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="I17" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
+      <c r="C18" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B18,FIND(" ",B18)),B18))</f>
         <v xml:space="preserve">SNP </v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H18">
+      <c r="I18" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
+      <c r="C19" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B19,FIND(" ",B19)),B19))</f>
         <v xml:space="preserve">SNG </v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H19">
+      <c r="I19" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
+      <c r="C20" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B20,FIND(" ",B20)),B20))</f>
         <v xml:space="preserve">JMP </v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H20">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="I20" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
+      <c r="C21" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B21,FIND(" ",B21)),B21))</f>
         <v xml:space="preserve">JMC </v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H21">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="I21" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
+      <c r="C22" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B22,FIND(" ",B22)),B22))</f>
         <v xml:space="preserve">JX </v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H22">
+      <c r="I22" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
+      <c r="C23" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B23,FIND(" ",B23)),B23))</f>
         <v xml:space="preserve">JME </v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H23">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="I23" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
+      <c r="C24" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B24,FIND(" ",B24)),B24))</f>
         <v xml:space="preserve">CALL </v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H24">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="I24" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
+      <c r="C25" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B25,FIND(" ",B25)),B25))</f>
         <v>RET</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H25">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="I25" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
+      <c r="C26" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B26,FIND(" ",B26)),B26))</f>
         <v xml:space="preserve">JMP </v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H26">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="I26" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
+      <c r="C27" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B27,FIND(" ",B27)),B27))</f>
         <v xml:space="preserve">CX </v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H27">
+      <c r="I27" s="5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
+      <c r="C28" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B28,FIND(" ",B28)),B28))</f>
         <v xml:space="preserve">CALL </v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H28">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="I28" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
+      <c r="C29" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B29,FIND(" ",B29)),B29))</f>
         <v xml:space="preserve">LDI </v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H29">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="I29" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
+      <c r="C30" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B30,FIND(" ",B30)),B30))</f>
         <v xml:space="preserve">LDI </v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H30">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="I30" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
+      <c r="C31" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B31,FIND(" ",B31)),B31))</f>
         <v xml:space="preserve">LDM </v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H31">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="I31" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
+      <c r="C32" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B32,FIND(" ",B32)),B32))</f>
         <v xml:space="preserve">LDM </v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H32">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="I32" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
+      <c r="C33" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B33,FIND(" ",B33)),B33))</f>
         <v xml:space="preserve">MOV </v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H33">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="I33" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
+      <c r="C34" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B34,FIND(" ",B34)),B34))</f>
         <v xml:space="preserve">STM </v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H34">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="I34" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C35" t="str">
-        <f t="shared" si="0"/>
+      <c r="C35" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B35,FIND(" ",B35)),B35))</f>
         <v xml:space="preserve">STM </v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H35">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="I35" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C36" t="str">
-        <f t="shared" si="0"/>
+      <c r="C36" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B36,FIND(" ",B36)),B36))</f>
         <v xml:space="preserve">ADDI </v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H36">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="I36" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
+      <c r="C37" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B37,FIND(" ",B37)),B37))</f>
         <v xml:space="preserve">ADD </v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H37">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="I37" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C38" t="str">
-        <f t="shared" si="0"/>
+      <c r="C38" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B38,FIND(" ",B38)),B38))</f>
         <v xml:space="preserve">ADD </v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H38">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="I38" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C39" t="str">
-        <f t="shared" si="0"/>
+      <c r="C39" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B39,FIND(" ",B39)),B39))</f>
         <v xml:space="preserve">SUBI </v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H39">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="I39" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C40" t="str">
-        <f t="shared" si="0"/>
+      <c r="C40" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B40,FIND(" ",B40)),B40))</f>
         <v xml:space="preserve">SUB </v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H40">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="I40" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C41" t="str">
-        <f t="shared" si="0"/>
+      <c r="C41" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B41,FIND(" ",B41)),B41))</f>
         <v xml:space="preserve">SUB </v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H41">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="I41" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C42" t="str">
-        <f t="shared" si="0"/>
+      <c r="C42" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B42,FIND(" ",B42)),B42))</f>
         <v xml:space="preserve">CMPI </v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H42">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="I42" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="str">
-        <f t="shared" si="0"/>
+      <c r="C43" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B43,FIND(" ",B43)),B43))</f>
         <v xml:space="preserve">CMP </v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H43">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="I43" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C44" t="str">
-        <f t="shared" si="0"/>
+      <c r="C44" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B44,FIND(" ",B44)),B44))</f>
         <v xml:space="preserve">ANDI </v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H44">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="I44" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C45" t="str">
-        <f t="shared" si="0"/>
+      <c r="C45" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B45,FIND(" ",B45)),B45))</f>
         <v xml:space="preserve">AND </v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H45">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="I45" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C46" t="str">
-        <f t="shared" si="0"/>
+      <c r="C46" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B46,FIND(" ",B46)),B46))</f>
         <v xml:space="preserve">AND </v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H46">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="I46" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C47" t="str">
-        <f t="shared" si="0"/>
+      <c r="C47" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B47,FIND(" ",B47)),B47))</f>
         <v xml:space="preserve">TSTI </v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H47">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="I47" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C48" t="str">
-        <f t="shared" si="0"/>
+      <c r="C48" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B48,FIND(" ",B48)),B48))</f>
         <v xml:space="preserve">TST </v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H48">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="I48" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C49" t="str">
-        <f t="shared" si="0"/>
+      <c r="C49" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B49,FIND(" ",B49)),B49))</f>
         <v xml:space="preserve">ORI </v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H49">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="I49" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C50" t="str">
-        <f t="shared" si="0"/>
+      <c r="C50" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B50,FIND(" ",B50)),B50))</f>
         <v xml:space="preserve">OR </v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H50">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="I50" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C51" t="str">
-        <f t="shared" si="0"/>
+      <c r="C51" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B51,FIND(" ",B51)),B51))</f>
         <v xml:space="preserve">OR </v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H51">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="I51" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C52" t="str">
-        <f t="shared" si="0"/>
+      <c r="C52" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B52,FIND(" ",B52)),B52))</f>
         <v xml:space="preserve">XORI </v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H52">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="I52" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C53" t="str">
-        <f t="shared" si="0"/>
+      <c r="C53" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B53,FIND(" ",B53)),B53))</f>
         <v xml:space="preserve">XOR </v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H53">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="I53" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C54" t="str">
-        <f t="shared" si="0"/>
+      <c r="C54" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B54,FIND(" ",B54)),B54))</f>
         <v xml:space="preserve">XOR </v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H54">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="I54" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C55" t="str">
-        <f t="shared" si="0"/>
+      <c r="C55" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B55,FIND(" ",B55)),B55))</f>
         <v xml:space="preserve">MULI </v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H55">
+      <c r="I55" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C56" t="str">
-        <f t="shared" si="0"/>
+      <c r="C56" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B56,FIND(" ",B56)),B56))</f>
         <v xml:space="preserve">MUL </v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H56">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="I56" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C57" t="str">
-        <f t="shared" si="0"/>
+      <c r="C57" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B57,FIND(" ",B57)),B57))</f>
         <v xml:space="preserve">MUL </v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H57">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="I57" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C58" t="str">
-        <f t="shared" si="0"/>
+      <c r="C58" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B58,FIND(" ",B58)),B58))</f>
         <v xml:space="preserve">DIVI </v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H58">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="I58" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C59" t="str">
-        <f t="shared" si="0"/>
+      <c r="C59" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B59,FIND(" ",B59)),B59))</f>
         <v xml:space="preserve">DIV </v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H59">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="I59" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C60" t="str">
-        <f t="shared" si="0"/>
+      <c r="C60" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B60,FIND(" ",B60)),B60))</f>
         <v xml:space="preserve">DIV </v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H60">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="I60" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C61" t="str">
-        <f t="shared" si="0"/>
+      <c r="C61" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B61,FIND(" ",B61)),B61))</f>
         <v xml:space="preserve">MODI </v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H61">
+      <c r="I61" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C62" t="str">
-        <f t="shared" si="0"/>
+      <c r="C62" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B62,FIND(" ",B62)),B62))</f>
         <v xml:space="preserve">MOD </v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H62">
+      <c r="I62" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C63" t="str">
-        <f t="shared" si="0"/>
+      <c r="C63" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B63,FIND(" ",B63)),B63))</f>
         <v xml:space="preserve">MOD </v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H63">
+      <c r="I63" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C64" t="str">
-        <f t="shared" si="0"/>
+      <c r="C64" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B64,FIND(" ",B64)),B64))</f>
         <v xml:space="preserve">REMI </v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G64" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H64">
+      <c r="I64" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C65" t="str">
-        <f t="shared" si="0"/>
+      <c r="C65" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B65,FIND(" ",B65)),B65))</f>
         <v xml:space="preserve">REM </v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G65" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H65">
+      <c r="I65" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C66" t="str">
-        <f t="shared" si="0"/>
+      <c r="C66" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B66,FIND(" ",B66)),B66))</f>
         <v xml:space="preserve">REM </v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H66">
+      <c r="I66" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C67" t="str">
-        <f t="shared" ref="C67:C88" si="1">UPPER(IFERROR(LEFT(B67,FIND(" ",B67)),B67))</f>
+      <c r="C67" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B67,FIND(" ",B67)),B67))</f>
         <v xml:space="preserve">SHL </v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H67">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="I67" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C68" t="str">
-        <f t="shared" si="1"/>
+      <c r="C68" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B68,FIND(" ",B68)),B68))</f>
         <v xml:space="preserve">SHR </v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H68">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="I68" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C69" t="str">
-        <f t="shared" si="1"/>
+      <c r="C69" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B69,FIND(" ",B69)),B69))</f>
         <v xml:space="preserve">SAL </v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G69" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H69">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="I69" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C70" t="str">
-        <f t="shared" si="1"/>
+      <c r="C70" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B70,FIND(" ",B70)),B70))</f>
         <v xml:space="preserve">SAR </v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G70" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H70">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="I70" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C71" t="str">
-        <f t="shared" si="1"/>
+      <c r="C71" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B71,FIND(" ",B71)),B71))</f>
         <v xml:space="preserve">SHL </v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G71" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H71">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="I71" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C72" t="str">
-        <f t="shared" si="1"/>
+      <c r="C72" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B72,FIND(" ",B72)),B72))</f>
         <v xml:space="preserve">SHR </v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G72" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H72">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="I72" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C73" t="str">
-        <f t="shared" si="1"/>
+      <c r="C73" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B73,FIND(" ",B73)),B73))</f>
         <v xml:space="preserve">SAL </v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H73">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="I73" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C74" t="str">
-        <f t="shared" si="1"/>
+      <c r="C74" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B74,FIND(" ",B74)),B74))</f>
         <v xml:space="preserve">SAR </v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G74" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H74">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="I74" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C75" t="str">
-        <f t="shared" si="1"/>
+      <c r="C75" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B75,FIND(" ",B75)),B75))</f>
         <v xml:space="preserve">PUSH </v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G75" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="H75">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="I75" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C76" t="str">
-        <f t="shared" si="1"/>
+      <c r="C76" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B76,FIND(" ",B76)),B76))</f>
         <v xml:space="preserve">POP </v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="H76">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="I76" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C77" t="str">
-        <f t="shared" si="1"/>
+      <c r="C77" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B77,FIND(" ",B77)),B77))</f>
         <v>PUSHALL</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="H77">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="I77" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C78" t="str">
-        <f t="shared" si="1"/>
+      <c r="C78" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B78,FIND(" ",B78)),B78))</f>
         <v>POPALL</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="H78">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="I78" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C79" t="str">
-        <f t="shared" si="1"/>
+      <c r="C79" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B79,FIND(" ",B79)),B79))</f>
         <v>PUSHF</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G79" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="H79">
+      <c r="I79" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="C80" t="str">
-        <f t="shared" si="1"/>
+      <c r="C80" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B80,FIND(" ",B80)),B80))</f>
         <v>POPF</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G80" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="H80">
+      <c r="I80" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C81" t="str">
-        <f t="shared" si="1"/>
+      <c r="C81" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B81,FIND(" ",B81)),B81))</f>
         <v xml:space="preserve">PAL </v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G81" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="H81">
+      <c r="I81" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C82" t="str">
-        <f t="shared" si="1"/>
+      <c r="C82" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B82,FIND(" ",B82)),B82))</f>
         <v xml:space="preserve">PAL </v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G82" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="H82">
+      <c r="I82" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="C83" t="str">
-        <f t="shared" si="1"/>
+      <c r="C83" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B83,FIND(" ",B83)),B83))</f>
         <v xml:space="preserve">NOTI </v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G83" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H83">
+      <c r="I83" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C84" t="str">
-        <f t="shared" si="1"/>
+      <c r="C84" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B84,FIND(" ",B84)),B84))</f>
         <v xml:space="preserve">NOT </v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G84" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H84">
+      <c r="I84" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C85" t="str">
-        <f t="shared" si="1"/>
+      <c r="C85" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B85,FIND(" ",B85)),B85))</f>
         <v xml:space="preserve">NOT </v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G85" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H85">
+      <c r="I85" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C86" t="str">
-        <f t="shared" si="1"/>
+      <c r="C86" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B86,FIND(" ",B86)),B86))</f>
         <v xml:space="preserve">NEGI </v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G86" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H86">
+      <c r="I86" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C87" t="str">
-        <f t="shared" si="1"/>
+      <c r="C87" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B87,FIND(" ",B87)),B87))</f>
         <v xml:space="preserve">NEG </v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="G87" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H87">
+      <c r="I87" s="5">
         <v>1.3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C88" t="str">
-        <f t="shared" si="1"/>
+      <c r="C88" s="5" t="str">
+        <f>UPPER(IFERROR(LEFT(B88,FIND(" ",B88)),B88))</f>
         <v xml:space="preserve">NEG </v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G88" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H88">
+      <c r="I88" s="5">
         <v>1.3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I88" xr:uid="{8C7AFE78-4A15-4265-94C1-6607B0A70F65}"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E1048576 F5:F7">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>